<commit_message>
collapse characteristics informality in a single coefficient
</commit_message>
<xml_diff>
--- a/Tables/reg_results/meanvardeps_period.xlsx
+++ b/Tables/reg_results/meanvardeps_period.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0"/>
@@ -13,47 +13,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="80" uniqueCount="33">
   <si>
     <t/>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Variable</t>
   </si>
   <si>
     <t>sex</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>eda</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>anios_esc</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>t_tra</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>casado</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>The value displayed for t-tests are the differences in the means across the groups.</t>
   </si>
   <si>
@@ -63,54 +45,18 @@
     <t>***, **, and * indicate significance at the 1, 5, and 10 percent critical level.</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
     <t>2.20e+09</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>2.20e+09</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>2.24e+09</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>2.24e+09</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>1.68e+09</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>(1)</t>
   </si>
   <si>
@@ -129,136 +75,49 @@
     <t>28.982</t>
   </si>
   <si>
-    <t>[0.000]</t>
-  </si>
-  <si>
     <t>6.088</t>
   </si>
   <si>
-    <t>[0.000]</t>
-  </si>
-  <si>
     <t>0.773</t>
   </si>
   <si>
-    <t>[0.000]</t>
-  </si>
-  <si>
     <t>0.536</t>
   </si>
   <si>
-    <t>[0.000]</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>2.83e+09</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>2.83e+09</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>2.87e+09</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>2.87e+09</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>2.21e+09</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>(2)</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>Mean/SE</t>
-  </si>
-  <si>
     <t>1.516</t>
   </si>
   <si>
-    <t>[0.000]</t>
-  </si>
-  <si>
     <t>30.500</t>
   </si>
   <si>
-    <t>[0.000]</t>
-  </si>
-  <si>
     <t>6.715</t>
   </si>
   <si>
-    <t>[0.000]</t>
-  </si>
-  <si>
     <t>0.793</t>
   </si>
   <si>
-    <t>[0.000]</t>
-  </si>
-  <si>
     <t>0.538</t>
-  </si>
-  <si>
-    <t>[0.000]</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -295,8 +154,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -304,271 +166,271 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>65</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>68</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>70</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>72</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>73</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>74</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>75</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>77</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>79</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>